<commit_message>
Algunos cambios no relevantes
</commit_message>
<xml_diff>
--- a/Backend/encuesta.xlsx
+++ b/Backend/encuesta.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Nombre Encuesta</t>
   </si>
@@ -29,36 +29,6 @@
   </si>
   <si>
     <t>Fecha Realización</t>
-  </si>
-  <si>
-    <t>¿Te gusta el almuerzo que recibes?</t>
-  </si>
-  <si>
-    <t>¿Cuántas veces comes al día?</t>
-  </si>
-  <si>
-    <t>Encuesta de Alimentación Escolar</t>
-  </si>
-  <si>
-    <t>form123</t>
-  </si>
-  <si>
-    <t>83749238592</t>
-  </si>
-  <si>
-    <t>Comedor Municipal 5</t>
-  </si>
-  <si>
-    <t>Juana</t>
-  </si>
-  <si>
-    <t>2024-10-01T10:30:00Z</t>
-  </si>
-  <si>
-    <t>Sí</t>
-  </si>
-  <si>
-    <t>3</t>
   </si>
 </sst>
 </file>
@@ -435,17 +405,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:F1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
     <col min="2" max="3" width="20" customWidth="1"/>
     <col min="4" max="5" width="25" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
-    <col min="7" max="8" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -463,38 +432,6 @@
       </c>
       <c r="F1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>